<commit_message>
Comments and Indexing added
</commit_message>
<xml_diff>
--- a/File_Generation/Output_Files/Final_Result.xlsx
+++ b/File_Generation/Output_Files/Final_Result.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D103"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,2250 +434,2556 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Gene Name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Alias1</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Alias2</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Alias3</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>deoA</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>VC_RS11310</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>VC2349</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>VC_2349</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>deoD</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>VC_RS13650</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>VCA0053</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>VC_A0053</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>fabA</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>VC_RS07175</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>VC1483</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>VC_1483</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>fabB</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>VC_RS10150</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>VC2109</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>VC_2109</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>fabD</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>VC_RS09735</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>VC2022</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>VC_2022</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>fadR</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>VC_RS09165</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>VC1900</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>VC_1900</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>fepB</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>VC_RS03890</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>VC0776</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>VC_0776</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>fis</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>VC_RS01410</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>VC0290</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>VC_0290</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>focA</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>VC_RS08205</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>VC1695</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>VC_1695</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>infA</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>VC_RS08390</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>VC1737</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>VC_1737</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>metK</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>VC_RS02420</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>VC0472</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>VC_0472</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>rplC</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>VC_RS12520</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>VC2596</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>VC_2596</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>rpmE</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>VC_RS12905</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>VC2679</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>VC_2679</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>rpsJ</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>VC_RS12525</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>VC2597</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>VC_2597</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>rrf</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>VC_RS13295</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>VC_r022</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>VCr022</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>rtxA</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>VC_RS07025</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>VC1451</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>VC_1451</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>rtxC</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>VC_RS07020</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>VC1450</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>VC_1450</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>tcpJ</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>VC_RS04175</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>VC0839</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>VC_0839</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
         <is>
           <t>VC_RS00275</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>VC_RS00275</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>VC_t001</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>VCt001</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
         <is>
           <t>VC_RS00740</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>VC_RS00740</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>VC_t004</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>VCt004</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
         <is>
           <t>VC_RS00755</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="C22" t="inlineStr">
         <is>
           <t>VC_RS00755</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>VC_t005</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>VCt005</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
         <is>
           <t>VC_RS01380</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>VC_RS01380</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>VC0284</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>VC_0284</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
         <is>
           <t>VC_RS01390</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>VC_RS01390</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>VC0286</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>VC_0286</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
         <is>
           <t>VC_RS01395</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>VC_RS01395</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>VC0287</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>VC_0287</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
         <is>
           <t>VC_RS01400</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>VC_RS01400</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>VC0288</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>VC_0288</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
         <is>
           <t>VC_RS01510</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>VC_RS01510</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>VC_t011</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>VCt011</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
         <is>
           <t>VC_RS01515</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="C28" t="inlineStr">
         <is>
           <t>VC_RS01515</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>VC_t012</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>VCt012</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
         <is>
           <t>VC_RS01945</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>VC_RS01945</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>VC_t026</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>VCt026</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
         <is>
           <t>VC_RS01950</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>VC_RS01950</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>VC_t027</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>VCt027</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
         <is>
           <t>VC_RS01965</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="C31" t="inlineStr">
         <is>
           <t>VC_RS01965</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>VC_t028</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="E31" t="inlineStr">
         <is>
           <t>VCt028</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
         <is>
           <t>VC_RS02265</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>VC_RS02265</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>VC_t030</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="E32" t="inlineStr">
         <is>
           <t>VCt030</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
         <is>
           <t>VC_RS02270</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>VC_RS02270</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>VC_t031</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t>VCt031</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
         <is>
           <t>VC_RS02275</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>VC_RS02275</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>VC_t032</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>VCt032</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
         <is>
           <t>VC_RS02295</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="C35" t="inlineStr">
         <is>
           <t>VC_RS02295</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>VC_t035</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="E35" t="inlineStr">
         <is>
           <t>VCt035</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
         <is>
           <t>VC_RS02435</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>VC_RS02435</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>VC0475</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="E36" t="inlineStr">
         <is>
           <t>VC_0475</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
         <is>
           <t>VC_RS03130</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>VC_RS03130</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>VC0618</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>VC_0618</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
         <is>
           <t>VC_RS03585</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>VC_RS03585</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>VC_t049</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="E38" t="inlineStr">
         <is>
           <t>VCt049</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
         <is>
           <t>VC_RS03600</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="C39" t="inlineStr">
         <is>
           <t>VC_RS03600</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>VC_t050</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="E39" t="inlineStr">
         <is>
           <t>VCt050</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
         <is>
           <t>VC_RS03860</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>VC_RS03860</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>VC0770</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="E40" t="inlineStr">
         <is>
           <t>VC_0770</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
         <is>
           <t>VC_RS03870</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="C41" t="inlineStr">
         <is>
           <t>VC_RS03870</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>VC0772</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="E41" t="inlineStr">
         <is>
           <t>VC_0772</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
         <is>
           <t>VC_RS03875</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>VC_RS03875</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="D42" t="inlineStr">
         <is>
           <t>VC0773</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="E42" t="inlineStr">
         <is>
           <t>VC_0773</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
         <is>
           <t>VC_RS05280</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="C43" t="inlineStr">
         <is>
           <t>VC_RS05280</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="D43" t="inlineStr">
         <is>
           <t>VC1074</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="E43" t="inlineStr">
         <is>
           <t>VC_1074</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
         <is>
           <t>VC_RS05840</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="C44" t="inlineStr">
         <is>
           <t>VC_RS05840</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>VC1193</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="E44" t="inlineStr">
         <is>
           <t>VC_1193</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
         <is>
           <t>VC_RS05880</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="C45" t="inlineStr">
         <is>
           <t>VC_RS05880</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="D45" t="inlineStr">
         <is>
           <t>VC1201</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="E45" t="inlineStr">
         <is>
           <t>VC_1201</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
         <is>
           <t>VC_RS06165</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="C46" t="inlineStr">
         <is>
           <t>VC_RS06165</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>VC1264</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="E46" t="inlineStr">
         <is>
           <t>VC_1264</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
         <is>
           <t>VC_RS06170</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="C47" t="inlineStr">
         <is>
           <t>VC_RS06170</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="D47" t="inlineStr">
         <is>
           <t>VC1265</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="E47" t="inlineStr">
         <is>
           <t>VC_1265</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
         <is>
           <t>VC_RS06205</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="C48" t="inlineStr">
         <is>
           <t>VC_RS06205</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="D48" t="inlineStr">
         <is>
           <t>VC1272</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="E48" t="inlineStr">
         <is>
           <t>VC_1272</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
         <is>
           <t>VC_RS06335</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="C49" t="inlineStr">
         <is>
           <t>VC_RS06335</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>VC1300</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="E49" t="inlineStr">
         <is>
           <t>VC_1300</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
         <is>
           <t>VC_RS06340</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="C50" t="inlineStr">
         <is>
           <t>VC_RS06340</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="D50" t="inlineStr">
         <is>
           <t>VC1301</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="E50" t="inlineStr">
         <is>
           <t>VC_1301</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
         <is>
           <t>VC_RS07015</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="C51" t="inlineStr">
         <is>
           <t>VC_RS07015</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="D51" t="inlineStr">
         <is>
           <t>VC1449</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="E51" t="inlineStr">
         <is>
           <t>VC_1449</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
         <is>
           <t>VC_RS07530</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
+      <c r="C52" t="inlineStr">
         <is>
           <t>VC_RS07530</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="D52" t="inlineStr">
         <is>
           <t>VC1556</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
+      <c r="E52" t="inlineStr">
         <is>
           <t>VC_1556</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
         <is>
           <t>VC_RS07535</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
+      <c r="C53" t="inlineStr">
         <is>
           <t>VC_RS07535</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="D53" t="inlineStr">
         <is>
           <t>VC1557</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
+      <c r="E53" t="inlineStr">
         <is>
           <t>VC_1557</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
         <is>
           <t>VC_RS07540</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
+      <c r="C54" t="inlineStr">
         <is>
           <t>VC_RS07540</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="D54" t="inlineStr">
         <is>
           <t>VC1558</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
+      <c r="E54" t="inlineStr">
         <is>
           <t>VC_1558</t>
         </is>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
         <is>
           <t>VC_RS08270</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="C55" t="inlineStr">
         <is>
           <t>VC_RS08270</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
+      <c r="D55" t="inlineStr">
         <is>
           <t>VC1709</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
+      <c r="E55" t="inlineStr">
         <is>
           <t>VC_1709</t>
         </is>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
         <is>
           <t>VC_RS09740</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
+      <c r="C56" t="inlineStr">
         <is>
           <t>VC_RS09740</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="D56" t="inlineStr">
         <is>
           <t>VC2023</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
+      <c r="E56" t="inlineStr">
         <is>
           <t>VC_2023</t>
         </is>
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
         <is>
           <t>VC_RS10315</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="C57" t="inlineStr">
         <is>
           <t>VC_RS10315</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="D57" t="inlineStr">
         <is>
           <t>VC2143</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
+      <c r="E57" t="inlineStr">
         <is>
           <t>VC_2143</t>
         </is>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
         <is>
           <t>VC_RS10495</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
+      <c r="C58" t="inlineStr">
         <is>
           <t>VC_RS10495</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="D58" t="inlineStr">
         <is>
           <t>VC_t066</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
+      <c r="E58" t="inlineStr">
         <is>
           <t>VCt066</t>
         </is>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
         <is>
           <t>VC_RS10500</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr">
+      <c r="C59" t="inlineStr">
         <is>
           <t>VC_RS10500</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
+      <c r="D59" t="inlineStr">
         <is>
           <t>VC_t067</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr">
+      <c r="E59" t="inlineStr">
         <is>
           <t>VCt067</t>
         </is>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
         <is>
           <t>VC_RS10505</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr">
+      <c r="C60" t="inlineStr">
         <is>
           <t>VC_RS10505</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
+      <c r="D60" t="inlineStr">
         <is>
           <t>VC_t068</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
+      <c r="E60" t="inlineStr">
         <is>
           <t>VCt068</t>
         </is>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
         <is>
           <t>VC_RS10510</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr">
+      <c r="C61" t="inlineStr">
         <is>
           <t>VC_RS10510</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
+      <c r="D61" t="inlineStr">
         <is>
           <t>VC_t069</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr">
+      <c r="E61" t="inlineStr">
         <is>
           <t>VCt069</t>
         </is>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
         <is>
           <t>VC_RS10515</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
+      <c r="C62" t="inlineStr">
         <is>
           <t>VC_RS10515</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
+      <c r="D62" t="inlineStr">
         <is>
           <t>VC_t070</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr">
+      <c r="E62" t="inlineStr">
         <is>
           <t>VCt070</t>
         </is>
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
         <is>
           <t>VC_RS10525</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr">
+      <c r="C63" t="inlineStr">
         <is>
           <t>VC_RS10525</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
+      <c r="D63" t="inlineStr">
         <is>
           <t>VC_t072</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
+      <c r="E63" t="inlineStr">
         <is>
           <t>VCt072</t>
         </is>
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
         <is>
           <t>VC_RS10690</t>
         </is>
       </c>
-      <c r="B64" t="inlineStr">
+      <c r="C64" t="inlineStr">
         <is>
           <t>VC_RS10690</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr">
+      <c r="D64" t="inlineStr">
         <is>
           <t>VC2211</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
+      <c r="E64" t="inlineStr">
         <is>
           <t>VC_2211</t>
         </is>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
         <is>
           <t>VC_RS11135</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr">
+      <c r="C65" t="inlineStr">
         <is>
           <t>VC_RS11135</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
+      <c r="D65" t="inlineStr">
         <is>
           <t>VC2305</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr">
+      <c r="E65" t="inlineStr">
         <is>
           <t>VC_2305</t>
         </is>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
         <is>
           <t>VC_RS11320</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
+      <c r="C66" t="inlineStr">
         <is>
           <t>VC_RS11320</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
+      <c r="D66" t="inlineStr">
         <is>
           <t>VC_2351</t>
         </is>
       </c>
-      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="inlineStr"/>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
         <is>
           <t>VC_RS12035</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
+      <c r="C67" t="inlineStr">
         <is>
           <t>VC_RS12035</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr">
+      <c r="D67" t="inlineStr">
         <is>
           <t>VC_t084</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr">
+      <c r="E67" t="inlineStr">
         <is>
           <t>VCt084</t>
         </is>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
         <is>
           <t>VC_RS12040</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
+      <c r="C68" t="inlineStr">
         <is>
           <t>VC_RS12040</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr">
+      <c r="D68" t="inlineStr">
         <is>
           <t>VC_t085</t>
         </is>
       </c>
-      <c r="D68" t="inlineStr">
+      <c r="E68" t="inlineStr">
         <is>
           <t>VCt085</t>
         </is>
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
         <is>
           <t>VC_RS12995</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
+      <c r="C69" t="inlineStr">
         <is>
           <t>VC_RS12995</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
+      <c r="D69" t="inlineStr">
         <is>
           <t>VC2699</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr">
+      <c r="E69" t="inlineStr">
         <is>
           <t>VC_2699</t>
         </is>
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
         <is>
           <t>VC_RS13270</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
+      <c r="C70" t="inlineStr">
         <is>
           <t>VC_RS13270</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
+      <c r="D70" t="inlineStr">
         <is>
           <t>VC_t088</t>
         </is>
       </c>
-      <c r="D70" t="inlineStr">
+      <c r="E70" t="inlineStr">
         <is>
           <t>VCt088</t>
         </is>
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
         <is>
           <t>VC_RS13305</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
+      <c r="C71" t="inlineStr">
         <is>
           <t>VC_RS13305</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
+      <c r="D71" t="inlineStr">
         <is>
           <t>VC_t092</t>
         </is>
       </c>
-      <c r="D71" t="inlineStr">
+      <c r="E71" t="inlineStr">
         <is>
           <t>VCt092</t>
         </is>
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="inlineStr">
         <is>
           <t>VC_RS13645</t>
         </is>
       </c>
-      <c r="B72" t="inlineStr">
+      <c r="C72" t="inlineStr">
         <is>
           <t>VC_RS13645</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
+      <c r="D72" t="inlineStr">
         <is>
           <t>VCA0052</t>
         </is>
       </c>
-      <c r="D72" t="inlineStr">
+      <c r="E72" t="inlineStr">
         <is>
           <t>VC_A0052</t>
         </is>
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="inlineStr">
         <is>
           <t>VC_RS13685</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr">
+      <c r="C73" t="inlineStr">
         <is>
           <t>VC_RS13685</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="D73" t="inlineStr">
         <is>
           <t>VCA0063</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr">
+      <c r="E73" t="inlineStr">
         <is>
           <t>VC_A0063</t>
         </is>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
         <is>
           <t>VC_RS13690</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
+      <c r="C74" t="inlineStr">
         <is>
           <t>VC_RS13690</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
+      <c r="D74" t="inlineStr">
         <is>
           <t>VCA0064</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr">
+      <c r="E74" t="inlineStr">
         <is>
           <t>VC_A0064</t>
         </is>
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
         <is>
           <t>VC_RS13695</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr">
+      <c r="C75" t="inlineStr">
         <is>
           <t>VC_RS13695</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr">
+      <c r="D75" t="inlineStr">
         <is>
           <t>VCA0065</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr">
+      <c r="E75" t="inlineStr">
         <is>
           <t>VC_A0065</t>
         </is>
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
         <is>
           <t>VC_RS13700</t>
         </is>
       </c>
-      <c r="B76" t="inlineStr">
+      <c r="C76" t="inlineStr">
         <is>
           <t>VC_RS13700</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr">
+      <c r="D76" t="inlineStr">
         <is>
           <t>VCA0066</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr">
+      <c r="E76" t="inlineStr">
         <is>
           <t>VC_A0066</t>
         </is>
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
         <is>
           <t>VC_RS13705</t>
         </is>
       </c>
-      <c r="B77" t="inlineStr">
+      <c r="C77" t="inlineStr">
         <is>
           <t>VC_RS13705</t>
         </is>
       </c>
-      <c r="C77" t="inlineStr">
+      <c r="D77" t="inlineStr">
         <is>
           <t>VCA0067</t>
         </is>
       </c>
-      <c r="D77" t="inlineStr">
+      <c r="E77" t="inlineStr">
         <is>
           <t>VC_A0067</t>
         </is>
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
         <is>
           <t>VC_RS14070</t>
         </is>
       </c>
-      <c r="B78" t="inlineStr">
+      <c r="C78" t="inlineStr">
         <is>
           <t>VC_RS14070</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr">
+      <c r="D78" t="inlineStr">
         <is>
           <t>VCA0150</t>
         </is>
       </c>
-      <c r="D78" t="inlineStr">
+      <c r="E78" t="inlineStr">
         <is>
           <t>VC_A0150</t>
         </is>
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
         <is>
           <t>VC_RS14205</t>
         </is>
       </c>
-      <c r="B79" t="inlineStr">
+      <c r="C79" t="inlineStr">
         <is>
           <t>VC_RS14205</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr">
+      <c r="D79" t="inlineStr">
         <is>
           <t>VCA0179</t>
         </is>
       </c>
-      <c r="D79" t="inlineStr">
+      <c r="E79" t="inlineStr">
         <is>
           <t>VC_A0179</t>
         </is>
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
         <is>
           <t>VC_RS14420</t>
         </is>
       </c>
-      <c r="B80" t="inlineStr">
+      <c r="C80" t="inlineStr">
         <is>
           <t>VC_RS14420</t>
         </is>
       </c>
-      <c r="C80" t="inlineStr">
+      <c r="D80" t="inlineStr">
         <is>
           <t>VCA0227</t>
         </is>
       </c>
-      <c r="D80" t="inlineStr">
+      <c r="E80" t="inlineStr">
         <is>
           <t>VC_A0227</t>
         </is>
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
         <is>
           <t>VC_RS14425</t>
         </is>
       </c>
-      <c r="B81" t="inlineStr">
+      <c r="C81" t="inlineStr">
         <is>
           <t>VC_RS14425</t>
         </is>
       </c>
-      <c r="C81" t="inlineStr">
+      <c r="D81" t="inlineStr">
         <is>
           <t>VCA0228</t>
         </is>
       </c>
-      <c r="D81" t="inlineStr">
+      <c r="E81" t="inlineStr">
         <is>
           <t>VC_A0228</t>
         </is>
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="inlineStr">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
         <is>
           <t>VC_RS14430</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr">
+      <c r="C82" t="inlineStr">
         <is>
           <t>VC_RS14430</t>
         </is>
       </c>
-      <c r="C82" t="inlineStr">
+      <c r="D82" t="inlineStr">
         <is>
           <t>VCA0229</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr">
+      <c r="E82" t="inlineStr">
         <is>
           <t>VC_A0229</t>
         </is>
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
         <is>
           <t>VC_RS15260</t>
         </is>
       </c>
-      <c r="B83" t="inlineStr">
+      <c r="C83" t="inlineStr">
         <is>
           <t>VC_RS15260</t>
         </is>
       </c>
-      <c r="C83" t="inlineStr"/>
       <c r="D83" t="inlineStr"/>
+      <c r="E83" t="inlineStr"/>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="inlineStr">
         <is>
           <t>VC_RS15335</t>
         </is>
       </c>
-      <c r="B84" t="inlineStr">
+      <c r="C84" t="inlineStr">
         <is>
           <t>VC_RS15335</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr">
+      <c r="D84" t="inlineStr">
         <is>
           <t>VCA0407</t>
         </is>
       </c>
-      <c r="D84" t="inlineStr">
+      <c r="E84" t="inlineStr">
         <is>
           <t>VC_A0407</t>
         </is>
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="inlineStr">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="inlineStr">
         <is>
           <t>VC_RS15360</t>
         </is>
       </c>
-      <c r="B85" t="inlineStr">
+      <c r="C85" t="inlineStr">
         <is>
           <t>VC_RS15360</t>
         </is>
       </c>
-      <c r="C85" t="inlineStr">
+      <c r="D85" t="inlineStr">
         <is>
           <t>VCA0412</t>
         </is>
       </c>
-      <c r="D85" t="inlineStr">
+      <c r="E85" t="inlineStr">
         <is>
           <t>VC_A0412</t>
         </is>
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="inlineStr">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="inlineStr">
         <is>
           <t>VC_RS16165</t>
         </is>
       </c>
-      <c r="B86" t="inlineStr">
+      <c r="C86" t="inlineStr">
         <is>
           <t>VC_RS16165</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr">
+      <c r="D86" t="inlineStr">
         <is>
           <t>VCA0576</t>
         </is>
       </c>
-      <c r="D86" t="inlineStr">
+      <c r="E86" t="inlineStr">
         <is>
           <t>VC_A0576</t>
         </is>
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="inlineStr">
         <is>
           <t>VC_RS16535</t>
         </is>
       </c>
-      <c r="B87" t="inlineStr">
+      <c r="C87" t="inlineStr">
         <is>
           <t>VC_RS16535</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr">
+      <c r="D87" t="inlineStr">
         <is>
           <t>VCA0658</t>
         </is>
       </c>
-      <c r="D87" t="inlineStr">
+      <c r="E87" t="inlineStr">
         <is>
           <t>VC_A0658</t>
         </is>
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="inlineStr">
         <is>
           <t>VC_RS16955</t>
         </is>
       </c>
-      <c r="B88" t="inlineStr">
+      <c r="C88" t="inlineStr">
         <is>
           <t>VC_RS16955</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr">
+      <c r="D88" t="inlineStr">
         <is>
           <t>VCA0754</t>
         </is>
       </c>
-      <c r="D88" t="inlineStr">
+      <c r="E88" t="inlineStr">
         <is>
           <t>VC_A0754</t>
         </is>
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="inlineStr">
         <is>
           <t>VC_RS16965</t>
         </is>
       </c>
-      <c r="B89" t="inlineStr">
+      <c r="C89" t="inlineStr">
         <is>
           <t>VC_RS16965</t>
         </is>
       </c>
-      <c r="C89" t="inlineStr">
+      <c r="D89" t="inlineStr">
         <is>
           <t>VCAt3</t>
         </is>
       </c>
-      <c r="D89" t="inlineStr">
+      <c r="E89" t="inlineStr">
         <is>
           <t>VC_At3</t>
         </is>
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="inlineStr">
         <is>
           <t>VC_RS17045</t>
         </is>
       </c>
-      <c r="B90" t="inlineStr">
+      <c r="C90" t="inlineStr">
         <is>
           <t>VC_RS17045</t>
         </is>
       </c>
-      <c r="C90" t="inlineStr">
+      <c r="D90" t="inlineStr">
         <is>
           <t>VCA0772</t>
         </is>
       </c>
-      <c r="D90" t="inlineStr">
+      <c r="E90" t="inlineStr">
         <is>
           <t>VC_A0772</t>
         </is>
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="inlineStr">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="inlineStr">
         <is>
           <t>VC_RS17430</t>
         </is>
       </c>
-      <c r="B91" t="inlineStr">
+      <c r="C91" t="inlineStr">
         <is>
           <t>VC_RS17430</t>
         </is>
       </c>
-      <c r="C91" t="inlineStr">
+      <c r="D91" t="inlineStr">
         <is>
           <t>VCA0862</t>
         </is>
       </c>
-      <c r="D91" t="inlineStr">
+      <c r="E91" t="inlineStr">
         <is>
           <t>VC_A0862</t>
         </is>
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="inlineStr">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="inlineStr">
         <is>
           <t>VC_RS17435</t>
         </is>
       </c>
-      <c r="B92" t="inlineStr">
+      <c r="C92" t="inlineStr">
         <is>
           <t>VC_RS17435</t>
         </is>
       </c>
-      <c r="C92" t="inlineStr">
+      <c r="D92" t="inlineStr">
         <is>
           <t>VCA0863</t>
         </is>
       </c>
-      <c r="D92" t="inlineStr">
+      <c r="E92" t="inlineStr">
         <is>
           <t>VC_A0863</t>
         </is>
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="inlineStr">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="inlineStr">
         <is>
           <t>VC_RS17490</t>
         </is>
       </c>
-      <c r="B93" t="inlineStr">
+      <c r="C93" t="inlineStr">
         <is>
           <t>VC_RS17490</t>
         </is>
       </c>
-      <c r="C93" t="inlineStr">
+      <c r="D93" t="inlineStr">
         <is>
           <t>VCA0874</t>
         </is>
       </c>
-      <c r="D93" t="inlineStr">
+      <c r="E93" t="inlineStr">
         <is>
           <t>VC_A0874</t>
         </is>
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="inlineStr">
         <is>
           <t>VC_RS17670</t>
         </is>
       </c>
-      <c r="B94" t="inlineStr">
+      <c r="C94" t="inlineStr">
         <is>
           <t>VC_RS17670</t>
         </is>
       </c>
-      <c r="C94" t="inlineStr">
+      <c r="D94" t="inlineStr">
         <is>
           <t>VCA0911</t>
         </is>
       </c>
-      <c r="D94" t="inlineStr">
+      <c r="E94" t="inlineStr">
         <is>
           <t>VC_A0911</t>
         </is>
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="inlineStr">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="inlineStr">
         <is>
           <t>VC_RS17675</t>
         </is>
       </c>
-      <c r="B95" t="inlineStr">
+      <c r="C95" t="inlineStr">
         <is>
           <t>VC_RS17675</t>
         </is>
       </c>
-      <c r="C95" t="inlineStr">
+      <c r="D95" t="inlineStr">
         <is>
           <t>VCA0912</t>
         </is>
       </c>
-      <c r="D95" t="inlineStr">
+      <c r="E95" t="inlineStr">
         <is>
           <t>VC_A0912</t>
         </is>
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="inlineStr">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="inlineStr">
         <is>
           <t>VC_RS17685</t>
         </is>
       </c>
-      <c r="B96" t="inlineStr">
+      <c r="C96" t="inlineStr">
         <is>
           <t>VC_RS17685</t>
         </is>
       </c>
-      <c r="C96" t="inlineStr">
+      <c r="D96" t="inlineStr">
         <is>
           <t>VCA0914</t>
         </is>
       </c>
-      <c r="D96" t="inlineStr">
+      <c r="E96" t="inlineStr">
         <is>
           <t>VC_A0914</t>
         </is>
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="inlineStr">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="inlineStr">
         <is>
           <t>VC_RS17765</t>
         </is>
       </c>
-      <c r="B97" t="inlineStr">
+      <c r="C97" t="inlineStr">
         <is>
           <t>VC_RS17765</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr">
+      <c r="D97" t="inlineStr">
         <is>
           <t>VCA0933</t>
         </is>
       </c>
-      <c r="D97" t="inlineStr">
+      <c r="E97" t="inlineStr">
         <is>
           <t>VC_A0933</t>
         </is>
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="inlineStr">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="inlineStr">
         <is>
           <t>VC_RS17950</t>
         </is>
       </c>
-      <c r="B98" t="inlineStr">
+      <c r="C98" t="inlineStr">
         <is>
           <t>VC_RS17950</t>
         </is>
       </c>
-      <c r="C98" t="inlineStr">
+      <c r="D98" t="inlineStr">
         <is>
           <t>VCA0976</t>
         </is>
       </c>
-      <c r="D98" t="inlineStr">
+      <c r="E98" t="inlineStr">
         <is>
           <t>VC_A0976</t>
         </is>
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="inlineStr">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="inlineStr">
         <is>
           <t>VC_RS18125</t>
         </is>
       </c>
-      <c r="B99" t="inlineStr">
+      <c r="C99" t="inlineStr">
         <is>
           <t>VC_RS18125</t>
         </is>
       </c>
-      <c r="C99" t="inlineStr">
+      <c r="D99" t="inlineStr">
         <is>
           <t>VCA1013</t>
         </is>
       </c>
-      <c r="D99" t="inlineStr">
+      <c r="E99" t="inlineStr">
         <is>
           <t>VC_A1013</t>
         </is>
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="inlineStr">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="inlineStr">
         <is>
           <t>VC_RS18620</t>
         </is>
       </c>
-      <c r="B100" t="inlineStr">
+      <c r="C100" t="inlineStr">
         <is>
           <t>VC_RS18620</t>
         </is>
       </c>
-      <c r="C100" t="inlineStr">
+      <c r="D100" t="inlineStr">
         <is>
           <t>VC_2753</t>
         </is>
       </c>
-      <c r="D100" t="inlineStr"/>
+      <c r="E100" t="inlineStr"/>
     </row>
     <row r="101">
-      <c r="A101" t="inlineStr">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="inlineStr">
         <is>
           <t>vesC</t>
         </is>
       </c>
-      <c r="B101" t="inlineStr">
+      <c r="C101" t="inlineStr">
         <is>
           <t>VC_RS07980</t>
         </is>
       </c>
-      <c r="C101" t="inlineStr">
+      <c r="D101" t="inlineStr">
         <is>
           <t>VC1649</t>
         </is>
       </c>
-      <c r="D101" t="inlineStr">
+      <c r="E101" t="inlineStr">
         <is>
           <t>VC_1649</t>
         </is>
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="inlineStr">
+      <c r="A102" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" t="inlineStr">
         <is>
           <t>vibB</t>
         </is>
       </c>
-      <c r="B102" t="inlineStr">
+      <c r="C102" t="inlineStr">
         <is>
           <t>VC_RS03865</t>
         </is>
       </c>
-      <c r="C102" t="inlineStr">
+      <c r="D102" t="inlineStr">
         <is>
           <t>VC0771</t>
         </is>
       </c>
-      <c r="D102" t="inlineStr">
+      <c r="E102" t="inlineStr">
         <is>
           <t>VC_0771</t>
         </is>
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="inlineStr">
+      <c r="A103" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" t="inlineStr">
         <is>
           <t>vibH</t>
         </is>
       </c>
-      <c r="B103" t="inlineStr">
+      <c r="C103" t="inlineStr">
         <is>
           <t>VC_RS03885</t>
         </is>
       </c>
-      <c r="C103" t="inlineStr">
+      <c r="D103" t="inlineStr">
         <is>
           <t>VC0775</t>
         </is>
       </c>
-      <c r="D103" t="inlineStr">
+      <c r="E103" t="inlineStr">
         <is>
           <t>VC_0775</t>
         </is>

</xml_diff>